<commit_message>
Added a motor and camera spec
</commit_message>
<xml_diff>
--- a/Datasheets/Electrical Project USST/BOM_Cable.xlsx
+++ b/Datasheets/Electrical Project USST/BOM_Cable.xlsx
@@ -20,12 +20,12 @@
     <sheet name="Antenna" sheetId="13" r:id="rId11"/>
     <sheet name="Misc" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
   <si>
     <t>Manufacturer No.</t>
   </si>
@@ -563,7 +563,13 @@
     <t>Optical Sensor Development Tools Time of Flight Distance SNSR</t>
   </si>
   <si>
-    <t>DRV8871 Motor Controller/Driver Power Management Evaluation Board</t>
+    <t>supplier number</t>
+  </si>
+  <si>
+    <t>1528-1020-ND</t>
+  </si>
+  <si>
+    <t>TRINKET MINI MCU BOARD 3.3V</t>
   </si>
 </sst>
 </file>
@@ -650,12 +656,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -680,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -725,9 +737,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3374,18 +3389,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3393,179 +3408,183 @@
         <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1386</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
       <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
         <v>49.61</v>
       </c>
-      <c r="G3" s="5">
-        <f>E3*F3</f>
+      <c r="H3" s="5">
+        <f>F3*G3</f>
         <v>49.61</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5">
+    <row r="4" spans="1:9" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>132</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>15.48</v>
       </c>
-      <c r="G4" s="5">
-        <f>E4*F4</f>
+      <c r="H4" s="5">
+        <f>F4*G4</f>
         <v>46.44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="25.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:9" ht="25.5">
+      <c r="A5" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="23">
         <v>20.66</v>
       </c>
-      <c r="G5" s="5">
-        <f>E5*F5</f>
+      <c r="H5" s="25">
+        <f>F5*G5</f>
         <v>20.66</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25.5">
+    <row r="6" spans="1:9" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>132</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>15.48</v>
       </c>
-      <c r="G6" s="5">
-        <f>E6*F6</f>
+      <c r="H6" s="5">
+        <f>F6*G6</f>
         <v>15.48</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>3317</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>21.93</v>
       </c>
-      <c r="G7" s="5">
-        <f>E7*F7</f>
+      <c r="H7" s="5">
+        <f>F7*G7</f>
         <v>21.93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="24">
-      <c r="A8" s="9">
-        <v>3190</v>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>1500</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
-      <c r="C8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+      <c r="C8" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>173</v>
       </c>
       <c r="F8">
-        <v>10.53</v>
-      </c>
-      <c r="G8" s="5">
-        <f>E8*F8</f>
-        <v>10.53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="D10" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>9.76</v>
+      </c>
+      <c r="H8" s="5">
+        <f>F8*G8</f>
+        <v>9.76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>